<commit_message>
asesoria 01 de octubre
</commit_message>
<xml_diff>
--- a/anexos/Estado de la cuestión Juan Calpa, Cristhian Padilla.xlsx
+++ b/anexos/Estado de la cuestión Juan Calpa, Cristhian Padilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorio\trabajo-de-grado-\anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE21F32-6324-4850-9A11-69D7AB4F386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A826D5-E7D5-4FC6-BCD8-A5BAA7B8209A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -964,6 +964,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -981,33 +1008,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -29765,46 +29765,46 @@
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -29819,26 +29819,26 @@
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -29856,13 +29856,13 @@
       <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -29870,67 +29870,67 @@
         <v>70</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -29945,40 +29945,40 @@
       <c r="E12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -29996,13 +29996,13 @@
       <c r="F15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="8" t="s">
@@ -30010,67 +30010,67 @@
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="94.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -30096,7 +30096,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="8" t="s">
         <v>70</v>
       </c>
@@ -30111,18 +30111,30 @@
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="A12:A13"/>
@@ -30137,18 +30149,6 @@
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B23" r:id="rId1" xr:uid="{06A3115A-1DC9-4848-B29A-C321974DCA5A}"/>
@@ -30179,46 +30179,46 @@
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -30233,26 +30233,26 @@
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="8"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -30270,13 +30270,13 @@
       <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8" t="s">
         <v>70</v>
@@ -30286,67 +30286,67 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -30361,40 +30361,40 @@
       <c r="E12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -30412,13 +30412,13 @@
       <c r="F15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
@@ -30426,67 +30426,67 @@
         <v>70</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -30512,7 +30512,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="8" t="s">
         <v>70</v>
       </c>
@@ -30527,30 +30527,18 @@
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="A12:A13"/>
@@ -30565,6 +30553,18 @@
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B23" r:id="rId1" xr:uid="{958F6A29-6789-4A27-845C-AFD1EFDFEFD7}"/>
@@ -30596,46 +30596,46 @@
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -30650,26 +30650,26 @@
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -30687,13 +30687,13 @@
       <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -30701,67 +30701,67 @@
         <v>70</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -30776,40 +30776,40 @@
       <c r="E12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -30827,81 +30827,81 @@
       <c r="F15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="27"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -30927,7 +30927,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="8" t="s">
         <v>70</v>
       </c>
@@ -30942,18 +30942,30 @@
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="A12:A13"/>
@@ -30968,18 +30980,6 @@
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B23" r:id="rId1" xr:uid="{D6663CD1-BA9E-44A4-8B92-139F79375522}"/>
@@ -31012,46 +31012,46 @@
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -31066,28 +31066,28 @@
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="8"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -31105,13 +31105,13 @@
       <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8" t="s">
         <v>70</v>
@@ -31119,67 +31119,67 @@
       <c r="D7" s="8"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -31194,40 +31194,40 @@
       <c r="E12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -31245,81 +31245,81 @@
       <c r="F15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="27"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -31345,7 +31345,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
       <c r="D22" s="8" t="s">
@@ -31360,30 +31360,18 @@
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="A12:A13"/>
@@ -31398,6 +31386,18 @@
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B23" r:id="rId1" xr:uid="{2C7E88CD-4F29-477C-8053-58AE35A9B153}"/>
@@ -31433,26 +31433,26 @@
       <c r="B1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -31461,15 +31461,15 @@
       <c r="B3" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -31484,26 +31484,26 @@
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -31521,13 +31521,13 @@
       <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="8" t="s">
@@ -31535,67 +31535,67 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -31610,40 +31610,40 @@
       <c r="E12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -31661,13 +31661,13 @@
       <c r="F15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="8" t="s">
@@ -31675,67 +31675,67 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -31761,7 +31761,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -31776,30 +31776,18 @@
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="A12:A13"/>
@@ -31814,6 +31802,18 @@
     <mergeCell ref="B19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B23" r:id="rId1" xr:uid="{317E717B-A32B-4455-8F31-46AC4478125A}"/>
@@ -31850,12 +31850,12 @@
       <c r="B1" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -31879,15 +31879,15 @@
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -31914,12 +31914,12 @@
       <c r="B3" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -31940,7 +31940,7 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -31955,11 +31955,11 @@
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -31980,16 +31980,16 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -32010,7 +32010,7 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -32028,10 +32028,10 @@
       <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -32052,7 +32052,7 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="8" t="s">
@@ -32060,8 +32060,8 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -32085,15 +32085,15 @@
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -32117,15 +32117,15 @@
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -32149,15 +32149,15 @@
       <c r="A10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -32180,15 +32180,15 @@
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -32209,7 +32209,7 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -32224,11 +32224,11 @@
       <c r="E12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -32249,16 +32249,16 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="9" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -32285,12 +32285,12 @@
       <c r="B14" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -32311,7 +32311,7 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -32329,10 +32329,10 @@
       <c r="F15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="19"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -32353,16 +32353,16 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="27"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -32386,15 +32386,15 @@
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -32418,15 +32418,15 @@
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -32450,15 +32450,15 @@
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -32482,15 +32482,15 @@
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -32511,7 +32511,7 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -32555,7 +32555,7 @@
       <c r="Z21" s="4"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="8" t="s">
         <v>70</v>
       </c>
@@ -32588,15 +32588,15 @@
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -57146,16 +57146,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
@@ -57172,6 +57162,16 @@
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B23" r:id="rId1" xr:uid="{97622EC6-5B10-4685-8838-BA744C09EBAD}"/>
@@ -57186,8 +57186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D38BBF-0B54-4DB6-BB3D-A83DDEE17D29}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -57199,8 +57199,8 @@
     <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">

</xml_diff>